<commit_message>
Add user-agent header and week 44 questions
</commit_message>
<xml_diff>
--- a/src/main/resources/weeklyQuestions.xlsx
+++ b/src/main/resources/weeklyQuestions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Week</t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>https://www.hackerrank.com/challenges/superman-celebrates-diwali/problem</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/strplay/problem</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/arithmetic-expressions/problem</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/array-construction/problem</t>
   </si>
 </sst>
 </file>
@@ -1773,6 +1782,30 @@
         <v>130</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" s="8">
+        <v>44.0</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="8">
+        <v>44.0</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="8">
+        <v>44.0</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -1904,7 +1937,10 @@
     <hyperlink r:id="rId127" ref="B128"/>
     <hyperlink r:id="rId128" ref="B129"/>
     <hyperlink r:id="rId129" ref="B130"/>
+    <hyperlink r:id="rId130" ref="B131"/>
+    <hyperlink r:id="rId131" ref="B132"/>
+    <hyperlink r:id="rId132" ref="B133"/>
   </hyperlinks>
-  <drawing r:id="rId130"/>
+  <drawing r:id="rId133"/>
 </worksheet>
 </file>
</xml_diff>